<commit_message>
add IDSheet; ensure that numbers are text
</commit_message>
<xml_diff>
--- a/AdvancedRepeatForm_import_test_01.xlsx
+++ b/AdvancedRepeatForm_import_test_01.xlsx
@@ -1,35 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tino/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="38160" windowHeight="18640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300"/>
   </bookViews>
   <sheets>
     <sheet name="Advanced Repeat Form" sheetId="1" r:id="rId1"/>
     <sheet name="group_cooking" sheetId="2" r:id="rId2"/>
     <sheet name="group_pets" sheetId="3" r:id="rId3"/>
+    <sheet name="IDSheet" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
   <si>
     <t>start</t>
   </si>
@@ -61,15 +57,6 @@
     <t>Preferred_Toppings</t>
   </si>
   <si>
-    <t>Last_Haircut</t>
-  </si>
-  <si>
-    <t>Haircut_before_last</t>
-  </si>
-  <si>
-    <t>Three_haircuts_ago</t>
-  </si>
-  <si>
     <t>__version__</t>
   </si>
   <si>
@@ -353,16 +340,53 @@
   </si>
   <si>
     <t>66</t>
+  </si>
+  <si>
+    <t>afRmyXNV6NeAtcXYs3fNaD</t>
+  </si>
+  <si>
+    <t>bb97d983300345d88748e629139f3062</t>
+  </si>
+  <si>
+    <t>KPI ID</t>
+  </si>
+  <si>
+    <t>KC ID</t>
+  </si>
+  <si>
+    <t>group_recent_haircuts::Last_Haircut</t>
+  </si>
+  <si>
+    <t>group_recent_haircuts::Haircut_before_last</t>
+  </si>
+  <si>
+    <t>group_recent_haircuts::Three_haircuts_ago</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -385,14 +409,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,7 +476,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -483,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -695,10 +723,10 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
@@ -718,7 +746,7 @@
     <col min="18" max="18" width="6.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,272 +778,278 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="O2" s="1">
         <v>7457138</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="O3" s="1">
         <v>7478651</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O4" s="1">
         <v>7480909</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1027,7 +1061,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1037,148 +1071,153 @@
     <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1190,7 +1229,7 @@
       <selection activeCell="F1" sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1200,127 +1239,171 @@
     <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA47" sqref="AA47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>